<commit_message>
Updated to publish toolbox PR1 for review
Added overview in new folder. Placed previous public review links on a new archive page. Updated the comments matrix for the toolboxes.
</commit_message>
<xml_diff>
--- a/comment/BIO-iTC-CommentsMatrix.xlsx
+++ b/comment/BIO-iTC-CommentsMatrix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\be.wood\Documents\GitHub\cPP-biometrics\4_Methodology\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\be.wood\Documents\GitHub\biometricITC\biometricITC.github.io\comment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Section</t>
   </si>
@@ -184,11 +184,27 @@
     <t>TB</t>
   </si>
   <si>
+    <t>Face</t>
+  </si>
+  <si>
+    <t>Eye</t>
+  </si>
+  <si>
+    <t>Finger</t>
+  </si>
+  <si>
+    <t>Vein</t>
+  </si>
+  <si>
     <t>The specific document the comments are for should be selected in G1. The fields are:
 - cPP - for the PP-Module
 - CFG - for the PP-Configuration
 - SD - for the Supporting Document
-- TB - for the PAD Toolbox overview</t>
+- TB - for the PAD Toolbox overview
+- Eye - for the Eye Toolbox
+- Face - for the Face Toolbox
+- Finger - for the Fingerprint Toolbox
+- Vein - for the Vein Toolbox</t>
   </si>
 </sst>
 </file>
@@ -483,8 +499,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="H7:H11" totalsRowShown="0">
-  <autoFilter ref="H7:H11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="H7:H15" totalsRowShown="0">
+  <autoFilter ref="H7:H15"/>
   <tableColumns count="1">
     <tableColumn id="1" name="DOCUMENT"/>
   </tableColumns>
@@ -1049,7 +1065,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Instructions!$H$8:$H$11</xm:f>
+            <xm:f>Instructions!$H$8:$H$15</xm:f>
           </x14:formula1>
           <xm:sqref>G1</xm:sqref>
         </x14:dataValidation>
@@ -1061,7 +1077,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -1079,12 +1095,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1160,6 +1176,26 @@
       </c>
       <c r="H11" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>